<commit_message>
Fixed wire stubs, updated BOM
</commit_message>
<xml_diff>
--- a/battery_monitoring_board/V2_2018_2019/Battery_Monitoring_V2_BOM.xlsx
+++ b/battery_monitoring_board/V2_2018_2019/Battery_Monitoring_V2_BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="142">
   <si>
     <t>Shematic Reference Number</t>
   </si>
@@ -270,9 +270,6 @@
     <t>JP4</t>
   </si>
   <si>
-    <t>J1-J8</t>
-  </si>
-  <si>
     <t>JP5</t>
   </si>
   <si>
@@ -436,13 +433,25 @@
   </si>
   <si>
     <t>Q7, Q8, Q9</t>
+  </si>
+  <si>
+    <t>We have these parts on hand</t>
+  </si>
+  <si>
+    <t>Part appears in multiple lists on this board</t>
+  </si>
+  <si>
+    <t>On hand</t>
+  </si>
+  <si>
+    <t>J1-J9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -499,7 +508,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -523,26 +532,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -554,36 +543,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -637,9 +602,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -654,7 +617,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -664,12 +627,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -679,30 +636,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="2" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -986,33 +943,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G49"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
     <col min="2" max="2" width="63.6640625" customWidth="1"/>
     <col min="3" max="3" width="23.109375" customWidth="1"/>
     <col min="4" max="4" width="19.5546875" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" customWidth="1"/>
+    <col min="10" max="10" width="37" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1032,12 +991,15 @@
         <v>5</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>8</v>
@@ -1054,14 +1016,15 @@
       <c r="F3" s="1">
         <v>1</v>
       </c>
-      <c r="G3" s="1">
-        <f t="shared" ref="G3:G10" si="0">F3*E3</f>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1">
+        <f>(F3)*E3</f>
         <v>0.34799999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>11</v>
@@ -1078,14 +1041,15 @@
       <c r="F4" s="1">
         <v>1</v>
       </c>
-      <c r="G4" s="1">
-        <f t="shared" si="0"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1">
+        <f t="shared" ref="H4:H13" si="0">(F4)*E4</f>
         <v>0.48</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>13</v>
@@ -1102,14 +1066,15 @@
       <c r="F5" s="1">
         <v>2</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="1"/>
+      <c r="H5" s="1">
         <f t="shared" si="0"/>
         <v>9.4E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>16</v>
@@ -1126,14 +1091,15 @@
       <c r="F6" s="1">
         <v>2</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="1"/>
+      <c r="H6" s="1">
         <f t="shared" si="0"/>
         <v>6.2E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>18</v>
@@ -1150,14 +1116,15 @@
       <c r="F7" s="1">
         <v>1</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="1"/>
+      <c r="H7" s="1">
         <f t="shared" si="0"/>
         <v>3.4000000000000002E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>20</v>
@@ -1174,16 +1141,17 @@
       <c r="F8" s="1">
         <v>2</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="1"/>
+      <c r="H8" s="1">
         <f t="shared" si="0"/>
         <v>0.78</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B9" s="1" t="s">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9" s="18" t="s">
         <v>23</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -1198,14 +1166,17 @@
       <c r="F9" s="1">
         <v>2</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="18">
+        <v>4</v>
+      </c>
+      <c r="H9" s="1">
         <f t="shared" si="0"/>
         <v>1.36</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>26</v>
@@ -1222,19 +1193,23 @@
       <c r="F10" s="1">
         <v>1</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="1"/>
+      <c r="H10" s="1">
         <f t="shared" si="0"/>
         <v>2.0499999999999998</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="J10" s="15" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="17">
+      <c r="C11" s="11">
         <v>39281023</v>
       </c>
       <c r="D11" s="3" t="s">
@@ -1246,12 +1221,13 @@
       <c r="F11" s="1">
         <v>1</v>
       </c>
-      <c r="G11" s="1">
-        <f>F11*E11</f>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1">
+        <f t="shared" si="0"/>
         <v>0.83</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>82</v>
       </c>
@@ -1270,14 +1246,18 @@
       <c r="F12" s="1">
         <v>1</v>
       </c>
-      <c r="G12" s="1">
-        <f t="shared" ref="G12:G13" si="1">F12*E12</f>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1">
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="J12" s="16" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>34</v>
@@ -1294,23 +1274,25 @@
       <c r="F13" s="1">
         <v>2</v>
       </c>
-      <c r="G13" s="1">
-        <f t="shared" si="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1">
+        <f t="shared" si="0"/>
         <v>2.56</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="21" t="s">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="22"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="23"/>
-    </row>
-    <row r="16" spans="1:7">
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="22"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -1330,134 +1312,142 @@
         <v>5</v>
       </c>
       <c r="G16" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="4" t="s">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="1">
         <v>5.39</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F17" s="1">
         <v>2</v>
       </c>
-      <c r="G17" s="6">
-        <f>PRODUCT(E17:F17)</f>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1">
+        <f>(F17)*E17</f>
         <v>10.78</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="4" t="s">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="1">
         <v>2.5099999999999998</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F18" s="1">
         <v>4</v>
       </c>
-      <c r="G18" s="6">
-        <f>PRODUCT(E18,F18)</f>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1">
+        <f t="shared" ref="H18:H28" si="1">(F18)*E18</f>
         <v>10.039999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="4" t="s">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="1">
         <v>4.63</v>
       </c>
-      <c r="F19" s="9">
+      <c r="F19" s="1">
         <v>3</v>
       </c>
-      <c r="G19" s="6">
-        <f>PRODUCT(E19,F19)</f>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1">
+        <f t="shared" si="1"/>
         <v>13.89</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="4" t="s">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="1">
         <v>1.0900000000000001</v>
       </c>
-      <c r="F20" s="9">
+      <c r="F20" s="1">
         <v>3</v>
       </c>
-      <c r="G20" s="6">
-        <f t="shared" ref="G20" si="2">PRODUCT(E20:F20)</f>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1">
+        <f t="shared" si="1"/>
         <v>3.2700000000000005</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="4" t="s">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E21" s="1">
         <v>0.32</v>
       </c>
-      <c r="F21" s="9">
+      <c r="F21" s="1">
         <v>3</v>
       </c>
-      <c r="G21" s="6">
-        <f t="shared" ref="G21:G22" si="3">PRODUCT(E21,F21)</f>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1">
+        <f t="shared" si="1"/>
         <v>0.96</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="12" t="s">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="18" t="s">
         <v>53</v>
       </c>
       <c r="C22" s="1" t="s">
@@ -1466,182 +1456,195 @@
       <c r="D22" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E22" s="11">
+      <c r="E22" s="1">
         <v>0.14000000000000001</v>
       </c>
       <c r="F22" s="1">
         <v>2</v>
       </c>
-      <c r="G22" s="6">
-        <f t="shared" si="3"/>
+      <c r="G22" s="18">
+        <v>7</v>
+      </c>
+      <c r="H22" s="1">
+        <f t="shared" si="1"/>
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="7" t="s">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="D23" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="1">
         <v>0.15</v>
       </c>
-      <c r="F23" s="10">
+      <c r="F23" s="1">
         <v>3</v>
       </c>
-      <c r="G23" s="6">
-        <f t="shared" ref="G23" si="4">PRODUCT(E23:F23)</f>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1">
+        <f t="shared" si="1"/>
         <v>0.44999999999999996</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="7" t="s">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D24" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E24" s="8">
+      <c r="E24" s="1">
         <v>0.15</v>
       </c>
-      <c r="F24" s="10">
+      <c r="F24" s="1">
         <v>3</v>
       </c>
-      <c r="G24" s="6">
-        <f t="shared" ref="G24:G25" si="5">PRODUCT(E24,F24)</f>
+      <c r="G24" s="18">
+        <v>16</v>
+      </c>
+      <c r="H24" s="1">
+        <f t="shared" si="1"/>
         <v>0.44999999999999996</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="27" t="s">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B25" s="29" t="s">
+      <c r="B25" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="D25" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E25" s="8">
+      <c r="E25" s="1">
         <v>0.15</v>
       </c>
-      <c r="F25" s="10">
+      <c r="F25" s="1">
         <v>3</v>
       </c>
-      <c r="G25" s="6">
-        <f t="shared" si="5"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1">
+        <f t="shared" si="1"/>
         <v>0.44999999999999996</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="7" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="D26" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E26" s="8">
+      <c r="E26" s="1">
         <v>0.45</v>
       </c>
-      <c r="F26" s="10">
+      <c r="F26" s="1">
         <v>2</v>
       </c>
-      <c r="G26" s="6">
-        <f t="shared" ref="G26" si="6">PRODUCT(E26:F26)</f>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1">
+        <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="7" t="s">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C27" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="D27" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E27" s="8">
+      <c r="E27" s="1">
         <v>0.51</v>
       </c>
-      <c r="F27" s="19">
+      <c r="F27" s="1">
         <v>1</v>
       </c>
-      <c r="G27" s="6">
-        <f t="shared" ref="G27:G28" si="7">PRODUCT(E27,F27)</f>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1">
+        <f t="shared" si="1"/>
         <v>0.51</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>83</v>
+        <v>141</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C28" s="16">
+      <c r="C28" s="10">
         <v>1714955</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D28" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E28" s="18">
+      <c r="E28" s="9">
         <v>2.11</v>
       </c>
-      <c r="F28" s="15">
-        <v>6</v>
-      </c>
-      <c r="G28" s="1">
-        <f t="shared" si="7"/>
-        <v>12.66</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="25"/>
-      <c r="B29" s="25"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="25"/>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="A30" s="20" t="s">
-        <v>136</v>
-      </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-    </row>
-    <row r="31" spans="1:7">
+      <c r="F28" s="9">
+        <v>9</v>
+      </c>
+      <c r="G28" s="9"/>
+      <c r="H28" s="1">
+        <f t="shared" si="1"/>
+        <v>18.989999999999998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="12"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="12"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="B30" s="19"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="19"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>0</v>
       </c>
@@ -1661,21 +1664,24 @@
         <v>5</v>
       </c>
       <c r="G31" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="H31" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>95</v>
-      </c>
       <c r="D32" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E32" s="1">
         <v>9.23</v>
@@ -1683,23 +1689,24 @@
       <c r="F32" s="1">
         <v>1</v>
       </c>
-      <c r="G32" s="1">
-        <f t="shared" ref="G32:G39" si="8">F32*E32</f>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1">
+        <f>(F32)*E32</f>
         <v>9.23</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
-      <c r="A33" s="28" t="s">
-        <v>126</v>
-      </c>
-      <c r="B33" s="28" t="s">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="D33" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>98</v>
       </c>
       <c r="E33" s="1">
         <v>3.68</v>
@@ -1707,23 +1714,26 @@
       <c r="F33" s="1">
         <v>4</v>
       </c>
-      <c r="G33" s="1">
-        <f t="shared" si="8"/>
+      <c r="G33" s="18">
+        <v>3</v>
+      </c>
+      <c r="H33" s="1">
+        <f t="shared" ref="H33:H42" si="2">(F33)*E33</f>
         <v>14.72</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="C34" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="D34" s="3" t="s">
         <v>101</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>102</v>
       </c>
       <c r="E34" s="1">
         <v>0.93</v>
@@ -1731,23 +1741,24 @@
       <c r="F34" s="1">
         <v>2</v>
       </c>
-      <c r="G34" s="1">
-        <f t="shared" si="8"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1">
+        <f t="shared" si="2"/>
         <v>1.86</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="D35" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>105</v>
       </c>
       <c r="E35" s="1">
         <v>0.15</v>
@@ -1755,23 +1766,24 @@
       <c r="F35" s="1">
         <v>2</v>
       </c>
-      <c r="G35" s="1">
-        <f t="shared" si="8"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1">
+        <f t="shared" si="2"/>
         <v>0.3</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="D36" s="3" t="s">
         <v>107</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>108</v>
       </c>
       <c r="E36" s="1">
         <v>0.1</v>
@@ -1779,23 +1791,24 @@
       <c r="F36" s="1">
         <v>2</v>
       </c>
-      <c r="G36" s="1">
-        <f t="shared" si="8"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1">
+        <f t="shared" si="2"/>
         <v>0.2</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C37" s="2" t="s">
-        <v>110</v>
-      </c>
       <c r="D37" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E37" s="1">
         <v>0.1</v>
@@ -1803,23 +1816,24 @@
       <c r="F37" s="1">
         <v>2</v>
       </c>
-      <c r="G37" s="1">
-        <f t="shared" si="8"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1">
+        <f t="shared" si="2"/>
         <v>0.2</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="D38" s="3" t="s">
         <v>112</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>113</v>
       </c>
       <c r="E38" s="1">
         <v>0.25</v>
@@ -1827,23 +1841,24 @@
       <c r="F38" s="1">
         <v>1</v>
       </c>
-      <c r="G38" s="1">
-        <f t="shared" si="8"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1">
+        <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>115</v>
-      </c>
       <c r="D39" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E39" s="1">
         <v>0.1</v>
@@ -1851,23 +1866,24 @@
       <c r="F39" s="1">
         <v>2</v>
       </c>
-      <c r="G39" s="1">
-        <f t="shared" si="8"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1">
+        <f t="shared" si="2"/>
         <v>0.2</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="D40" s="3" t="s">
         <v>117</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>118</v>
       </c>
       <c r="E40" s="1">
         <v>0.27</v>
@@ -1875,23 +1891,24 @@
       <c r="F40" s="1">
         <v>5</v>
       </c>
-      <c r="G40" s="1">
-        <f>F40*E40</f>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1">
+        <f t="shared" si="2"/>
         <v>1.35</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B41" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="D41" s="3" t="s">
         <v>120</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>121</v>
       </c>
       <c r="E41" s="1">
         <v>0.34</v>
@@ -1899,47 +1916,50 @@
       <c r="F41" s="1">
         <v>1</v>
       </c>
-      <c r="G41" s="1">
-        <f t="shared" ref="G41:G42" si="9">F41*E41</f>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1">
+        <f t="shared" si="2"/>
         <v>0.34</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
-      <c r="A42" s="15" t="s">
-        <v>134</v>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42" s="9" t="s">
+        <v>133</v>
       </c>
       <c r="B42" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="D42" s="3" t="s">
         <v>123</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>124</v>
       </c>
       <c r="E42" s="1">
         <v>1.94</v>
       </c>
       <c r="F42" s="1">
-        <v>1</v>
-      </c>
-      <c r="G42" s="1">
-        <f t="shared" si="9"/>
-        <v>1.94</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7">
-      <c r="A44" s="24" t="s">
-        <v>135</v>
-      </c>
-      <c r="B44" s="24"/>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24"/>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24"/>
-      <c r="G44" s="24"/>
-    </row>
-    <row r="45" spans="1:7">
+        <v>0</v>
+      </c>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A44" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="B44" s="23"/>
+      <c r="C44" s="23"/>
+      <c r="D44" s="23"/>
+      <c r="E44" s="23"/>
+      <c r="F44" s="23"/>
+      <c r="G44" s="23"/>
+      <c r="H44" s="23"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>0</v>
       </c>
@@ -1959,45 +1979,49 @@
         <v>5</v>
       </c>
       <c r="G45" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="H45" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
-      <c r="A46" s="27" t="s">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E46" s="5">
+        <v>0.15</v>
+      </c>
+      <c r="F46" s="6">
+        <v>3</v>
+      </c>
+      <c r="G46" s="17"/>
+      <c r="H46" s="4">
+        <f t="shared" ref="H46" si="3">PRODUCT(E46,F46)</f>
+        <v>0.44999999999999996</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A47" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="B46" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="C46" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="D46" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="E46" s="8">
-        <v>0.15</v>
-      </c>
-      <c r="F46" s="10">
-        <v>3</v>
-      </c>
-      <c r="G46" s="6">
-        <f t="shared" ref="G46" si="10">PRODUCT(E46,F46)</f>
-        <v>0.44999999999999996</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7">
-      <c r="A47" s="28" t="s">
-        <v>138</v>
-      </c>
-      <c r="B47" s="28" t="s">
+      <c r="B47" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="D47" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>98</v>
       </c>
       <c r="E47" s="1">
         <v>3.68</v>
@@ -2005,26 +2029,28 @@
       <c r="F47" s="1">
         <v>3</v>
       </c>
-      <c r="G47" s="1">
-        <f t="shared" ref="G47" si="11">F47*E47</f>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1">
+        <f t="shared" ref="H47" si="4">F47*E47</f>
         <v>11.040000000000001</v>
       </c>
     </row>
-    <row r="49" spans="6:7">
-      <c r="F49" s="13" t="s">
+    <row r="49" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F49" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="G49" s="13">
-        <f>SUM(G3:G13,G17:G28,G32:G42,G46:G47)</f>
-        <v>105.51800000000001</v>
+      <c r="G49" s="7"/>
+      <c r="H49" s="7">
+        <f>SUM(H3:H13,H17:H28,H32:H42,H46:H47)</f>
+        <v>109.90800000000002</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A15:G15"/>
-    <mergeCell ref="A44:G44"/>
-    <mergeCell ref="A30:G30"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="A44:H44"/>
+    <mergeCell ref="A30:H30"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1"/>
@@ -2042,8 +2068,9 @@
     <hyperlink ref="D38" r:id="rId13"/>
     <hyperlink ref="D41" r:id="rId14"/>
     <hyperlink ref="D39" r:id="rId15"/>
+    <hyperlink ref="D28" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId16"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Given that there was a column listing total part numbers on hand I added an additional column to calculate how many parts needed to be purchased.
</commit_message>
<xml_diff>
--- a/battery_monitoring_board/V2_2018_2019/Battery_Monitoring_V2_BOM.xlsx
+++ b/battery_monitoring_board/V2_2018_2019/Battery_Monitoring_V2_BOM.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b59mi\Documents\Business\ARVP\au_hardware\battery_monitoring_board\V2_2018_2019\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9045"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="143">
   <si>
     <t>Shematic Reference Number</t>
   </si>
@@ -36,9 +41,6 @@
     <t>Price</t>
   </si>
   <si>
-    <t>Quantity</t>
-  </si>
-  <si>
     <t>Total Cost</t>
   </si>
   <si>
@@ -445,12 +447,18 @@
   </si>
   <si>
     <t>J1-J9</t>
+  </si>
+  <si>
+    <t>Quantity Required</t>
+  </si>
+  <si>
+    <t>Quantity To Buy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -935,7 +943,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -943,25 +951,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J49"/>
+  <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
-    <col min="2" max="2" width="63.6640625" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1"/>
-    <col min="4" max="4" width="19.5546875" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" customWidth="1"/>
-    <col min="10" max="10" width="37" customWidth="1"/>
+    <col min="2" max="2" width="63.7109375" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" customWidth="1"/>
+    <col min="11" max="11" width="37" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="19"/>
       <c r="C1" s="19"/>
@@ -970,8 +979,9 @@
       <c r="F1" s="19"/>
       <c r="G1" s="19"/>
       <c r="H1" s="19"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I1" s="19"/>
+    </row>
+    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -987,28 +997,31 @@
       <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>10</v>
       </c>
       <c r="E3" s="1">
         <v>0.34799999999999998</v>
@@ -1018,22 +1031,26 @@
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1">
+        <f>IF((F3-G3)&gt;0, F3-G3, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="I3" s="1">
         <f>(F3)*E3</f>
         <v>0.34799999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="D4" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" s="1">
         <v>0.48</v>
@@ -1043,22 +1060,26 @@
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1">
-        <f t="shared" ref="H4:H13" si="0">(F4)*E4</f>
+        <f t="shared" ref="H4:H13" si="0">IF((F4-G4)&gt;0, F4-G4, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="I4" s="1">
+        <f t="shared" ref="I4:I13" si="1">(F4)*E4</f>
         <v>0.48</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="E5" s="1">
         <v>4.7E-2</v>
@@ -1069,21 +1090,25 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1">
         <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I5" s="1">
+        <f t="shared" si="1"/>
         <v>9.4E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="D6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E6" s="1">
         <v>3.1E-2</v>
@@ -1094,21 +1119,25 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1">
         <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I6" s="1">
+        <f t="shared" si="1"/>
         <v>6.2E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="D7" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E7" s="1">
         <v>3.4000000000000002E-2</v>
@@ -1119,21 +1148,25 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1">
         <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I7" s="1">
+        <f t="shared" si="1"/>
         <v>3.4000000000000002E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="E8" s="1">
         <v>0.39</v>
@@ -1144,21 +1177,25 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1">
         <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I8" s="1">
+        <f t="shared" si="1"/>
         <v>0.78</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B9" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="E9" s="1">
         <v>0.68</v>
@@ -1171,21 +1208,25 @@
       </c>
       <c r="H9" s="1">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I9" s="1">
+        <f t="shared" si="1"/>
         <v>1.36</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="E10" s="1">
         <v>2.0499999999999998</v>
@@ -1196,24 +1237,28 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1">
         <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I10" s="1">
+        <f t="shared" si="1"/>
         <v>2.0499999999999998</v>
       </c>
-      <c r="J10" s="15" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K10" s="15" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" s="11">
         <v>39281023</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E11" s="1">
         <v>0.83</v>
@@ -1224,21 +1269,25 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1">
         <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I11" s="1">
+        <f t="shared" si="1"/>
         <v>0.83</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="E12" s="1">
         <v>0.2</v>
@@ -1249,24 +1298,28 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1">
         <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I12" s="1">
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
-      <c r="J12" s="16" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K12" s="16" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>36</v>
       </c>
       <c r="E13" s="1">
         <v>1.28</v>
@@ -1277,12 +1330,16 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1">
         <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I13" s="1">
+        <f t="shared" si="1"/>
         <v>2.56</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" s="21"/>
       <c r="C15" s="21"/>
@@ -1290,9 +1347,10 @@
       <c r="E15" s="21"/>
       <c r="F15" s="21"/>
       <c r="G15" s="21"/>
-      <c r="H15" s="22"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H15" s="21"/>
+      <c r="I15" s="22"/>
+    </row>
+    <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -1308,28 +1366,31 @@
       <c r="E16" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F16" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="I16" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E17" s="1">
         <v>5.39</v>
@@ -1339,22 +1400,26 @@
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1">
+        <f>IF((F17-G17)&gt;0, F17-G17, 0)</f>
+        <v>2</v>
+      </c>
+      <c r="I17" s="1">
         <f>(F17)*E17</f>
         <v>10.78</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="E18" s="1">
         <v>2.5099999999999998</v>
@@ -1364,22 +1429,26 @@
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1">
-        <f t="shared" ref="H18:H28" si="1">(F18)*E18</f>
+        <f t="shared" ref="H18:H28" si="2">IF((F18-G18)&gt;0, F18-G18, 0)</f>
+        <v>4</v>
+      </c>
+      <c r="I18" s="1">
+        <f t="shared" ref="I18:I28" si="3">(F18)*E18</f>
         <v>10.039999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E19" s="1">
         <v>4.63</v>
@@ -1389,22 +1458,26 @@
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="I19" s="1">
+        <f t="shared" si="3"/>
         <v>13.89</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="E20" s="1">
         <v>1.0900000000000001</v>
@@ -1414,22 +1487,26 @@
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="I20" s="1">
+        <f t="shared" si="3"/>
         <v>3.2700000000000005</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E21" s="1">
         <v>0.32</v>
@@ -1439,22 +1516,26 @@
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="I21" s="1">
+        <f t="shared" si="3"/>
         <v>0.96</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B22" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="E22" s="1">
         <v>0.14000000000000001</v>
@@ -1466,22 +1547,26 @@
         <v>7</v>
       </c>
       <c r="H22" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I22" s="1">
+        <f t="shared" si="3"/>
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="E23" s="1">
         <v>0.15</v>
@@ -1491,22 +1576,26 @@
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="I23" s="1">
+        <f t="shared" si="3"/>
         <v>0.44999999999999996</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B24" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="D24" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E24" s="1">
         <v>0.15</v>
@@ -1518,22 +1607,26 @@
         <v>16</v>
       </c>
       <c r="H24" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I24" s="1">
+        <f t="shared" si="3"/>
         <v>0.44999999999999996</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="D25" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E25" s="1">
         <v>0.15</v>
@@ -1543,22 +1636,26 @@
       </c>
       <c r="G25" s="1"/>
       <c r="H25" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="I25" s="1">
+        <f t="shared" si="3"/>
         <v>0.44999999999999996</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="E26" s="1">
         <v>0.45</v>
@@ -1568,22 +1665,26 @@
       </c>
       <c r="G26" s="1"/>
       <c r="H26" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="I26" s="1">
+        <f t="shared" si="3"/>
         <v>0.9</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E27" s="1">
         <v>0.51</v>
@@ -1593,22 +1694,26 @@
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="I27" s="1">
+        <f t="shared" si="3"/>
         <v>0.51</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C28" s="10">
         <v>1714955</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E28" s="9">
         <v>2.11</v>
@@ -1618,11 +1723,15 @@
       </c>
       <c r="G28" s="9"/>
       <c r="H28" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="I28" s="1">
+        <f t="shared" si="3"/>
         <v>18.989999999999998</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="12"/>
       <c r="B29" s="12"/>
       <c r="C29" s="13"/>
@@ -1630,11 +1739,12 @@
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
-      <c r="H29" s="12"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H29" s="8"/>
+      <c r="I29" s="12"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B30" s="19"/>
       <c r="C30" s="19"/>
@@ -1643,8 +1753,9 @@
       <c r="F30" s="19"/>
       <c r="G30" s="19"/>
       <c r="H30" s="19"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I30" s="19"/>
+    </row>
+    <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>0</v>
       </c>
@@ -1660,28 +1771,31 @@
       <c r="E31" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="F31" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="I31" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G31" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>94</v>
-      </c>
       <c r="D32" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E32" s="1">
         <v>9.23</v>
@@ -1691,22 +1805,26 @@
       </c>
       <c r="G32" s="1"/>
       <c r="H32" s="1">
+        <f t="shared" ref="H32:H42" si="4">IF((F32-G32)&gt;0, F32-G32, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="I32" s="1">
         <f>(F32)*E32</f>
         <v>9.23</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B33" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="D33" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>97</v>
       </c>
       <c r="E33" s="1">
         <v>3.68</v>
@@ -1718,22 +1836,26 @@
         <v>3</v>
       </c>
       <c r="H33" s="1">
-        <f t="shared" ref="H33:H42" si="2">(F33)*E33</f>
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="I33" s="1">
+        <f t="shared" ref="I33:I42" si="5">(F33)*E33</f>
         <v>14.72</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="C34" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="D34" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>101</v>
       </c>
       <c r="E34" s="1">
         <v>0.93</v>
@@ -1743,22 +1865,26 @@
       </c>
       <c r="G34" s="1"/>
       <c r="H34" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="I34" s="1">
+        <f t="shared" si="5"/>
         <v>1.86</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="D35" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>104</v>
       </c>
       <c r="E35" s="1">
         <v>0.15</v>
@@ -1768,22 +1894,26 @@
       </c>
       <c r="G35" s="1"/>
       <c r="H35" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="I35" s="1">
+        <f t="shared" si="5"/>
         <v>0.3</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="D36" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>107</v>
       </c>
       <c r="E36" s="1">
         <v>0.1</v>
@@ -1793,22 +1923,26 @@
       </c>
       <c r="G36" s="1"/>
       <c r="H36" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="I36" s="1">
+        <f t="shared" si="5"/>
         <v>0.2</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C37" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="D37" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E37" s="1">
         <v>0.1</v>
@@ -1818,22 +1952,26 @@
       </c>
       <c r="G37" s="1"/>
       <c r="H37" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="I37" s="1">
+        <f t="shared" si="5"/>
         <v>0.2</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="D38" s="3" t="s">
         <v>111</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>112</v>
       </c>
       <c r="E38" s="1">
         <v>0.25</v>
@@ -1843,22 +1981,26 @@
       </c>
       <c r="G38" s="1"/>
       <c r="H38" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="I38" s="1">
+        <f t="shared" si="5"/>
         <v>0.25</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>114</v>
-      </c>
       <c r="D39" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E39" s="1">
         <v>0.1</v>
@@ -1868,22 +2010,26 @@
       </c>
       <c r="G39" s="1"/>
       <c r="H39" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="I39" s="1">
+        <f t="shared" si="5"/>
         <v>0.2</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="D40" s="3" t="s">
         <v>116</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>117</v>
       </c>
       <c r="E40" s="1">
         <v>0.27</v>
@@ -1893,22 +2039,26 @@
       </c>
       <c r="G40" s="1"/>
       <c r="H40" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="I40" s="1">
+        <f t="shared" si="5"/>
         <v>1.35</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B41" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="D41" s="3" t="s">
         <v>119</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>120</v>
       </c>
       <c r="E41" s="1">
         <v>0.34</v>
@@ -1918,22 +2068,26 @@
       </c>
       <c r="G41" s="1"/>
       <c r="H41" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="I41" s="1">
+        <f t="shared" si="5"/>
         <v>0.34</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B42" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="D42" s="3" t="s">
         <v>122</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>123</v>
       </c>
       <c r="E42" s="1">
         <v>1.94</v>
@@ -1943,13 +2097,17 @@
       </c>
       <c r="G42" s="1"/>
       <c r="H42" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I42" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="23" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B44" s="23"/>
       <c r="C44" s="23"/>
@@ -1958,8 +2116,9 @@
       <c r="F44" s="23"/>
       <c r="G44" s="23"/>
       <c r="H44" s="23"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I44" s="23"/>
+    </row>
+    <row r="45" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>0</v>
       </c>
@@ -1975,28 +2134,31 @@
       <c r="E45" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F45" s="1" t="s">
+      <c r="F45" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="I45" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G45" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B46" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C46" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="C46" s="6" t="s">
-        <v>62</v>
-      </c>
       <c r="D46" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E46" s="5">
         <v>0.15</v>
@@ -2005,23 +2167,27 @@
         <v>3</v>
       </c>
       <c r="G46" s="17"/>
-      <c r="H46" s="4">
-        <f t="shared" ref="H46" si="3">PRODUCT(E46,F46)</f>
+      <c r="H46" s="1">
+        <f t="shared" ref="H46:H47" si="6">IF((F46-G46)&gt;0, F46-G46, 0)</f>
+        <v>3</v>
+      </c>
+      <c r="I46" s="4">
+        <f t="shared" ref="I46" si="7">PRODUCT(E46,F46)</f>
         <v>0.44999999999999996</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B47" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="D47" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>97</v>
       </c>
       <c r="E47" s="1">
         <v>3.68</v>
@@ -2031,26 +2197,31 @@
       </c>
       <c r="G47" s="1"/>
       <c r="H47" s="1">
-        <f t="shared" ref="H47" si="4">F47*E47</f>
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="I47" s="1">
+        <f t="shared" ref="I47" si="8">F47*E47</f>
         <v>11.040000000000001</v>
       </c>
     </row>
-    <row r="49" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F49" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G49" s="7"/>
-      <c r="H49" s="7">
-        <f>SUM(H3:H13,H17:H28,H32:H42,H46:H47)</f>
+      <c r="H49" s="7"/>
+      <c r="I49" s="7">
+        <f>SUM(I3:I13,I17:I28,I32:I42,I46:I47)</f>
         <v>109.90800000000002</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="A44:H44"/>
-    <mergeCell ref="A30:H30"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="A44:I44"/>
+    <mergeCell ref="A30:I30"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1"/>

</xml_diff>

<commit_message>
Added board name column for sorting purposes later.
</commit_message>
<xml_diff>
--- a/battery_monitoring_board/V2_2018_2019/Battery_Monitoring_V2_BOM.xlsx
+++ b/battery_monitoring_board/V2_2018_2019/Battery_Monitoring_V2_BOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="145">
   <si>
     <t>Shematic Reference Number</t>
   </si>
@@ -453,6 +453,12 @@
   </si>
   <si>
     <t>Quantity To Buy</t>
+  </si>
+  <si>
+    <t>Customer Reference</t>
+  </si>
+  <si>
+    <t>BATT_MON</t>
   </si>
 </sst>
 </file>
@@ -516,7 +522,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -618,6 +624,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -625,7 +642,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -653,9 +670,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -666,6 +680,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -953,8 +976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -965,21 +988,23 @@
     <col min="4" max="4" width="19.5703125" customWidth="1"/>
     <col min="6" max="6" width="9.85546875" customWidth="1"/>
     <col min="9" max="9" width="12.28515625" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" customWidth="1"/>
     <col min="11" max="11" width="37" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
     </row>
     <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1009,6 +1034,9 @@
       <c r="I2" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="J2" s="23" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -1038,6 +1066,9 @@
         <f>(F3)*E3</f>
         <v>0.34799999999999998</v>
       </c>
+      <c r="J3" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -1067,6 +1098,9 @@
         <f t="shared" ref="I4:I13" si="1">(F4)*E4</f>
         <v>0.48</v>
       </c>
+      <c r="J4" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -1096,6 +1130,9 @@
         <f t="shared" si="1"/>
         <v>9.4E-2</v>
       </c>
+      <c r="J5" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -1125,6 +1162,9 @@
         <f t="shared" si="1"/>
         <v>6.2E-2</v>
       </c>
+      <c r="J6" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1154,6 +1194,9 @@
         <f t="shared" si="1"/>
         <v>3.4000000000000002E-2</v>
       </c>
+      <c r="J7" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -1183,6 +1226,9 @@
         <f t="shared" si="1"/>
         <v>0.78</v>
       </c>
+      <c r="J8" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
@@ -1214,6 +1260,9 @@
         <f t="shared" si="1"/>
         <v>1.36</v>
       </c>
+      <c r="J9" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -1243,6 +1292,9 @@
         <f t="shared" si="1"/>
         <v>2.0499999999999998</v>
       </c>
+      <c r="J10" s="1" t="s">
+        <v>144</v>
+      </c>
       <c r="K10" s="15" t="s">
         <v>138</v>
       </c>
@@ -1275,6 +1327,9 @@
         <f t="shared" si="1"/>
         <v>0.83</v>
       </c>
+      <c r="J11" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -1304,6 +1359,9 @@
         <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
+      <c r="J12" s="1" t="s">
+        <v>144</v>
+      </c>
       <c r="K12" s="16" t="s">
         <v>137</v>
       </c>
@@ -1336,19 +1394,23 @@
         <f t="shared" si="1"/>
         <v>2.56</v>
       </c>
+      <c r="J13" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="22"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="21"/>
     </row>
     <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -1378,8 +1440,11 @@
       <c r="I16" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16" s="23" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>70</v>
       </c>
@@ -1407,8 +1472,11 @@
         <f>(F17)*E17</f>
         <v>10.78</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>71</v>
       </c>
@@ -1436,8 +1504,11 @@
         <f t="shared" ref="I18:I28" si="3">(F18)*E18</f>
         <v>10.039999999999999</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>72</v>
       </c>
@@ -1465,8 +1536,11 @@
         <f t="shared" si="3"/>
         <v>13.89</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>73</v>
       </c>
@@ -1494,8 +1568,11 @@
         <f t="shared" si="3"/>
         <v>3.2700000000000005</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>74</v>
       </c>
@@ -1523,8 +1600,11 @@
         <f t="shared" si="3"/>
         <v>0.96</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J21" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
         <v>75</v>
       </c>
@@ -1554,8 +1634,11 @@
         <f t="shared" si="3"/>
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>76</v>
       </c>
@@ -1583,8 +1666,11 @@
         <f t="shared" si="3"/>
         <v>0.44999999999999996</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J23" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
         <v>77</v>
       </c>
@@ -1614,8 +1700,11 @@
         <f t="shared" si="3"/>
         <v>0.44999999999999996</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J24" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>78</v>
       </c>
@@ -1643,8 +1732,11 @@
         <f t="shared" si="3"/>
         <v>0.44999999999999996</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J25" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>79</v>
       </c>
@@ -1672,8 +1764,11 @@
         <f t="shared" si="3"/>
         <v>0.9</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J26" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>80</v>
       </c>
@@ -1701,8 +1796,11 @@
         <f t="shared" si="3"/>
         <v>0.51</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J27" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>140</v>
       </c>
@@ -1730,8 +1828,11 @@
         <f t="shared" si="3"/>
         <v>18.989999999999998</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J28" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="12"/>
       <c r="B29" s="12"/>
       <c r="C29" s="13"/>
@@ -1742,20 +1843,21 @@
       <c r="H29" s="8"/>
       <c r="I29" s="12"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="B30" s="19"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="19"/>
-      <c r="I30" s="19"/>
-    </row>
-    <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="21"/>
+    </row>
+    <row r="31" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>0</v>
       </c>
@@ -1783,8 +1885,11 @@
       <c r="I31" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J31" s="23" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>123</v>
       </c>
@@ -1812,8 +1917,11 @@
         <f>(F32)*E32</f>
         <v>9.23</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J32" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
         <v>124</v>
       </c>
@@ -1843,8 +1951,11 @@
         <f t="shared" ref="I33:I42" si="5">(F33)*E33</f>
         <v>14.72</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J33" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>97</v>
       </c>
@@ -1872,8 +1983,11 @@
         <f t="shared" si="5"/>
         <v>1.86</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J34" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>125</v>
       </c>
@@ -1901,8 +2015,11 @@
         <f t="shared" si="5"/>
         <v>0.3</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J35" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>126</v>
       </c>
@@ -1930,8 +2047,11 @@
         <f t="shared" si="5"/>
         <v>0.2</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J36" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>127</v>
       </c>
@@ -1959,8 +2079,11 @@
         <f t="shared" si="5"/>
         <v>0.2</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J37" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>128</v>
       </c>
@@ -1988,8 +2111,11 @@
         <f t="shared" si="5"/>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J38" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>129</v>
       </c>
@@ -2017,8 +2143,11 @@
         <f t="shared" si="5"/>
         <v>0.2</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J39" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>130</v>
       </c>
@@ -2046,8 +2175,11 @@
         <f t="shared" si="5"/>
         <v>1.35</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J40" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>131</v>
       </c>
@@ -2075,8 +2207,11 @@
         <f t="shared" si="5"/>
         <v>0.34</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J41" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>132</v>
       </c>
@@ -2104,21 +2239,24 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="23" t="s">
+      <c r="J42" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="22" t="s">
         <v>133</v>
       </c>
-      <c r="B44" s="23"/>
-      <c r="C44" s="23"/>
-      <c r="D44" s="23"/>
-      <c r="E44" s="23"/>
-      <c r="F44" s="23"/>
-      <c r="G44" s="23"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-    </row>
-    <row r="45" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B44" s="22"/>
+      <c r="C44" s="22"/>
+      <c r="D44" s="22"/>
+      <c r="E44" s="22"/>
+      <c r="F44" s="22"/>
+      <c r="G44" s="22"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+    </row>
+    <row r="45" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>0</v>
       </c>
@@ -2146,8 +2284,11 @@
       <c r="I45" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J45" s="23" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>135</v>
       </c>
@@ -2175,8 +2316,11 @@
         <f t="shared" ref="I46" si="7">PRODUCT(E46,F46)</f>
         <v>0.44999999999999996</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J46" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
         <v>136</v>
       </c>
@@ -2203,6 +2347,9 @@
       <c r="I47" s="1">
         <f t="shared" ref="I47" si="8">F47*E47</f>
         <v>11.040000000000001</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="49" spans="6:9" x14ac:dyDescent="0.25">
@@ -2218,10 +2365,10 @@
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A15:I15"/>
     <mergeCell ref="A44:I44"/>
-    <mergeCell ref="A30:I30"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="A15:J15"/>
+    <mergeCell ref="A1:J1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1"/>

</xml_diff>